<commit_message>
Add script to retrieve data
</commit_message>
<xml_diff>
--- a/docs/supplementary/supplementary_table_1.xlsx
+++ b/docs/supplementary/supplementary_table_1.xlsx
@@ -8,144 +8,6 @@
   <definedNames/>
   <calcPr/>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="A42">
-      <text>
-        <t xml:space="preserve">https://ngs.arb-silva.de/silvangs/Index.html
-	-Christina P</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="AJ23">
-      <text>
-        <t xml:space="preserve">This is more of a data exchange platform, rather than a data analysis platform
-	-Christina P</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A41">
-      <text>
-        <t xml:space="preserve">https://seqera.io/
-	-Clea Siguret
-not finished
-	-Clea Siguret
-Why not just "seqera"?
-	-Christina P</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A15">
-      <text>
-        <t xml:space="preserve">https://labs.epi2me.io/
-	-Clea Siguret
-need to be check
-	-Clea Siguret
-I think this should be just  "EPI2ME"
-	-Christina P</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A29">
-      <text>
-        <t xml:space="preserve">https://mgx-metagenomics.github.io/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A33">
-      <text>
-        <t xml:space="preserve">https://mage.genoscope.cns.fr/microscope/home/index.php
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A34">
-      <text>
-        <t xml:space="preserve">http://microbial-genomes.org/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A32">
-      <text>
-        <t xml:space="preserve">https://micromap.icm.csic.es/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A17">
-      <text>
-        <t xml:space="preserve">https://services.bromberglab.org/fusiondb/mapping
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A11">
-      <text>
-        <t xml:space="preserve">https://www.uibk.ac.at/en/microbiology/services/coma/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A40">
-      <text>
-        <t xml:space="preserve">https://scata.mykopat.slu.se/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A30">
-      <text>
-        <t xml:space="preserve">https://www.microbiomeanalyst.ca/MicrobiomeAnalyst/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A16">
-      <text>
-        <t xml:space="preserve">https://web.rniapps.net/fungeco/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A23">
-      <text>
-        <t xml:space="preserve">https://www.imicrobe.us/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A19">
-      <text>
-        <t xml:space="preserve">https://gcmeta.wdcm.org/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A39">
-      <text>
-        <t xml:space="preserve">https://gauravsk.shinyapps.io/ranacapa/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A24">
-      <text>
-        <t xml:space="preserve">https://web.rniapps.net/iVikodak/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A10">
-      <text>
-        <t xml:space="preserve">https://cb.csail.mit.edu/carnelian/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A9">
-      <text>
-        <t xml:space="preserve">https://bugbase.cs.umn.edu
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A18">
-      <text>
-        <t xml:space="preserve">https://metagenomics.sequentiabiotech.com/gaia/
-	-Bérénice Batut</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59142,7 +59004,6 @@
       <formula1>"yes,no,in development"</formula1>
     </dataValidation>
   </dataValidations>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update data from codex
</commit_message>
<xml_diff>
--- a/docs/supplementary/supplementary_table_1.xlsx
+++ b/docs/supplementary/supplementary_table_1.xlsx
@@ -479,7 +479,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,6 +518,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
@@ -529,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -575,6 +581,18 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -586,6 +604,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -605,16 +626,16 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1474,19 +1495,19 @@
         <v>43</v>
       </c>
       <c r="W6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X6" s="9" t="s">
         <v>43</v>
       </c>
       <c r="Y6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z6" s="9" t="s">
         <v>44</v>
       </c>
       <c r="AA6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB6" s="9" t="s">
         <v>44</v>
@@ -1531,128 +1552,128 @@
       <c r="AZ6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="C7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="F7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="16">
         <v>45502.0</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="R7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="V7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="W7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="X7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ7" s="11"/>
-      <c r="AK7" s="11"/>
-      <c r="AL7" s="11"/>
-      <c r="AM7" s="11"/>
-      <c r="AN7" s="11"/>
-      <c r="AO7" s="11"/>
-      <c r="AP7" s="11"/>
-      <c r="AQ7" s="11"/>
-      <c r="AR7" s="11"/>
-      <c r="AS7" s="11"/>
-      <c r="AT7" s="11"/>
-      <c r="AU7" s="11"/>
-      <c r="AV7" s="11"/>
-      <c r="AW7" s="11"/>
-      <c r="AX7" s="11"/>
-      <c r="AY7" s="11"/>
-      <c r="AZ7" s="11"/>
+      <c r="K7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="V7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="W7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="X7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="18"/>
+      <c r="AM7" s="18"/>
+      <c r="AN7" s="18"/>
+      <c r="AO7" s="18"/>
+      <c r="AP7" s="18"/>
+      <c r="AQ7" s="18"/>
+      <c r="AR7" s="18"/>
+      <c r="AS7" s="18"/>
+      <c r="AT7" s="18"/>
+      <c r="AU7" s="18"/>
+      <c r="AV7" s="18"/>
+      <c r="AW7" s="18"/>
+      <c r="AX7" s="18"/>
+      <c r="AY7" s="18"/>
+      <c r="AZ7" s="18"/>
     </row>
     <row r="8">
       <c r="A8" s="14" t="s">
@@ -1987,19 +2008,19 @@
         <v>43</v>
       </c>
       <c r="AD10" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="AF10" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AG10" s="9" t="s">
         <v>44</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI10" s="9" t="s">
         <v>44</v>
@@ -2086,7 +2107,7 @@
         <v>43</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X11" s="9" t="s">
         <v>43</v>
@@ -2098,7 +2119,7 @@
         <v>43</v>
       </c>
       <c r="AA11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AB11" s="9" t="s">
         <v>44</v>
@@ -2110,10 +2131,10 @@
         <v>43</v>
       </c>
       <c r="AE11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AF11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AG11" s="9" t="s">
         <v>43</v>
@@ -2152,7 +2173,7 @@
       <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -2167,7 +2188,7 @@
       <c r="H12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J12" s="13">
@@ -2182,22 +2203,22 @@
       <c r="M12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q12" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="R12" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="S12" s="15" t="s">
+      <c r="N12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" s="19" t="s">
         <v>44</v>
       </c>
       <c r="T12" s="9" t="s">
@@ -2231,7 +2252,7 @@
         <v>44</v>
       </c>
       <c r="AD12" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE12" s="9" t="s">
         <v>44</v>
@@ -2248,7 +2269,7 @@
       <c r="AI12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AJ12" s="15"/>
+      <c r="AJ12" s="19"/>
       <c r="AK12" s="11"/>
       <c r="AL12" s="11"/>
       <c r="AM12" s="11"/>
@@ -2276,7 +2297,7 @@
       <c r="C13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="9"/>
@@ -2289,7 +2310,7 @@
       <c r="H13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J13" s="9">
@@ -2304,22 +2325,22 @@
       <c r="M13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="N13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q13" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="R13" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="S13" s="15" t="s">
+      <c r="N13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="19" t="s">
         <v>44</v>
       </c>
       <c r="T13" s="9" t="s">
@@ -2338,7 +2359,7 @@
         <v>43</v>
       </c>
       <c r="Y13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z13" s="9" t="s">
         <v>44</v>
@@ -2370,7 +2391,7 @@
       <c r="AI13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AJ13" s="15"/>
+      <c r="AJ13" s="19"/>
       <c r="AK13" s="11"/>
       <c r="AL13" s="11"/>
       <c r="AM13" s="11"/>
@@ -2398,7 +2419,7 @@
       <c r="C14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="9"/>
@@ -2411,7 +2432,7 @@
       <c r="H14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="19" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="9">
@@ -2426,25 +2447,25 @@
       <c r="M14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="R14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="S14" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="T14" s="15" t="s">
+      <c r="N14" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="T14" s="19" t="s">
         <v>44</v>
       </c>
       <c r="U14" s="10" t="s">
@@ -2481,7 +2502,7 @@
         <v>44</v>
       </c>
       <c r="AF14" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AG14" s="9" t="s">
         <v>43</v>
@@ -2492,7 +2513,7 @@
       <c r="AI14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AJ14" s="15"/>
+      <c r="AJ14" s="19"/>
       <c r="AK14" s="11"/>
       <c r="AL14" s="11"/>
       <c r="AM14" s="11"/>
@@ -2518,7 +2539,7 @@
       <c r="C15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -2533,10 +2554,10 @@
       <c r="H15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="16">
+      <c r="I15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="20">
         <v>45519.0</v>
       </c>
       <c r="K15" s="9" t="s">
@@ -2548,25 +2569,25 @@
       <c r="M15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="R15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="S15" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="T15" s="15" t="s">
+      <c r="N15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="T15" s="19" t="s">
         <v>44</v>
       </c>
       <c r="U15" s="10" t="s">
@@ -2614,7 +2635,7 @@
       <c r="AI15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AJ15" s="15" t="s">
+      <c r="AJ15" s="19" t="s">
         <v>73</v>
       </c>
       <c r="AK15" s="11"/>
@@ -2644,7 +2665,7 @@
       <c r="C16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="9"/>
@@ -2657,7 +2678,7 @@
       <c r="H16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="19" t="s">
         <v>44</v>
       </c>
       <c r="J16" s="9">
@@ -2672,25 +2693,25 @@
       <c r="M16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="N16" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="R16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="S16" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="T16" s="15" t="s">
+      <c r="N16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="T16" s="19" t="s">
         <v>44</v>
       </c>
       <c r="U16" s="10" t="s">
@@ -2738,7 +2759,7 @@
       <c r="AI16" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AJ16" s="15"/>
+      <c r="AJ16" s="19"/>
       <c r="AK16" s="11"/>
       <c r="AL16" s="11"/>
       <c r="AM16" s="11"/>
@@ -2902,7 +2923,7 @@
       <c r="I18" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="17"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="9" t="s">
         <v>44</v>
       </c>
@@ -2961,7 +2982,7 @@
         <v>44</v>
       </c>
       <c r="AD18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE18" s="9" t="s">
         <v>44</v>
@@ -3082,7 +3103,7 @@
         <v>43</v>
       </c>
       <c r="AD19" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE19" s="9" t="s">
         <v>44</v>
@@ -3121,7 +3142,7 @@
       <c r="A20" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="22" t="s">
         <v>83</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -3171,7 +3192,7 @@
         <v>43</v>
       </c>
       <c r="S20" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T20" s="9" t="s">
         <v>44</v>
@@ -3267,7 +3288,7 @@
       <c r="I21" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="17"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="9" t="s">
         <v>44</v>
       </c>
@@ -3296,7 +3317,7 @@
         <v>43</v>
       </c>
       <c r="T21" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U21" s="10" t="s">
         <v>44</v>
@@ -3362,126 +3383,126 @@
       <c r="AZ21" s="11"/>
     </row>
     <row r="22">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="13">
+      <c r="C22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="16">
         <v>45627.0</v>
       </c>
-      <c r="K22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="R22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="S22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="T22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="V22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="W22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="X22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI22" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ22" s="11"/>
-      <c r="AK22" s="11"/>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11"/>
-      <c r="AN22" s="11"/>
-      <c r="AO22" s="11"/>
-      <c r="AP22" s="11"/>
-      <c r="AQ22" s="11"/>
-      <c r="AR22" s="11"/>
-      <c r="AS22" s="11"/>
-      <c r="AT22" s="11"/>
-      <c r="AU22" s="11"/>
-      <c r="AV22" s="11"/>
-      <c r="AW22" s="11"/>
-      <c r="AX22" s="11"/>
-      <c r="AY22" s="11"/>
-      <c r="AZ22" s="11"/>
+      <c r="K22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="O22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="R22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="S22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="U22" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="V22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="W22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="X22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="18"/>
+      <c r="AL22" s="18"/>
+      <c r="AM22" s="18"/>
+      <c r="AN22" s="18"/>
+      <c r="AO22" s="18"/>
+      <c r="AP22" s="18"/>
+      <c r="AQ22" s="18"/>
+      <c r="AR22" s="18"/>
+      <c r="AS22" s="18"/>
+      <c r="AT22" s="18"/>
+      <c r="AU22" s="18"/>
+      <c r="AV22" s="18"/>
+      <c r="AW22" s="18"/>
+      <c r="AX22" s="18"/>
+      <c r="AY22" s="18"/>
+      <c r="AZ22" s="18"/>
     </row>
     <row r="23">
       <c r="A23" s="14" t="s">
@@ -3511,7 +3532,7 @@
       <c r="I23" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="17"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="9" t="s">
         <v>43</v>
       </c>
@@ -3540,10 +3561,10 @@
         <v>43</v>
       </c>
       <c r="T23" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V23" s="9" t="s">
         <v>43</v>
@@ -3558,7 +3579,7 @@
         <v>43</v>
       </c>
       <c r="Z23" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA23" s="9" t="s">
         <v>43</v>
@@ -3609,121 +3630,121 @@
       <c r="A24" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="J24" s="22"/>
-      <c r="K24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="O24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="P24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="R24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="S24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="T24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="U24" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="V24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="W24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="X24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ24" s="21"/>
-      <c r="AK24" s="21"/>
-      <c r="AL24" s="21"/>
-      <c r="AM24" s="21"/>
-      <c r="AN24" s="21"/>
-      <c r="AO24" s="21"/>
-      <c r="AP24" s="21"/>
-      <c r="AQ24" s="21"/>
-      <c r="AR24" s="21"/>
-      <c r="AS24" s="21"/>
-      <c r="AT24" s="21"/>
-      <c r="AU24" s="21"/>
-      <c r="AV24" s="21"/>
-      <c r="AW24" s="21"/>
-      <c r="AX24" s="21"/>
-      <c r="AY24" s="21"/>
-      <c r="AZ24" s="21"/>
+      <c r="C24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" s="27"/>
+      <c r="K24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="N24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="P24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="R24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="S24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="U24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="V24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="W24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="X24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH24" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI24" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ24" s="26"/>
+      <c r="AK24" s="26"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="26"/>
+      <c r="AN24" s="26"/>
+      <c r="AO24" s="26"/>
+      <c r="AP24" s="26"/>
+      <c r="AQ24" s="26"/>
+      <c r="AR24" s="26"/>
+      <c r="AS24" s="26"/>
+      <c r="AT24" s="26"/>
+      <c r="AU24" s="26"/>
+      <c r="AV24" s="26"/>
+      <c r="AW24" s="26"/>
+      <c r="AX24" s="26"/>
+      <c r="AY24" s="26"/>
+      <c r="AZ24" s="26"/>
     </row>
     <row r="25">
       <c r="A25" s="14" t="s">
@@ -3785,7 +3806,7 @@
         <v>43</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V25" s="9" t="s">
         <v>43</v>
@@ -3800,7 +3821,7 @@
         <v>43</v>
       </c>
       <c r="Z25" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AA25" s="9" t="s">
         <v>43</v>
@@ -3821,7 +3842,7 @@
         <v>43</v>
       </c>
       <c r="AG25" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AH25" s="9" t="s">
         <v>43</v>
@@ -4268,7 +4289,7 @@
         <v>44</v>
       </c>
       <c r="R29" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S29" s="9" t="s">
         <v>43</v>
@@ -4365,7 +4386,7 @@
       <c r="I30" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="24">
+      <c r="J30" s="29">
         <v>45590.0</v>
       </c>
       <c r="K30" s="9" t="s">
@@ -4462,124 +4483,124 @@
       <c r="AZ30" s="11"/>
     </row>
     <row r="31">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" s="25" t="s">
+      <c r="B31" s="31"/>
+      <c r="C31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="H31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="I31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J31" s="27"/>
-      <c r="K31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="L31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="N31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="O31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="P31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="R31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="S31" s="25" t="s">
+      <c r="F31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" s="32"/>
+      <c r="K31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="M31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="N31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="O31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="P31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S31" s="30" t="s">
         <v>43</v>
       </c>
       <c r="T31" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="U31" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="V31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="W31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="X31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AE31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH31" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI31" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ31" s="26"/>
-      <c r="AK31" s="26"/>
-      <c r="AL31" s="26"/>
-      <c r="AM31" s="26"/>
-      <c r="AN31" s="26"/>
-      <c r="AO31" s="26"/>
-      <c r="AP31" s="26"/>
-      <c r="AQ31" s="26"/>
-      <c r="AR31" s="26"/>
-      <c r="AS31" s="26"/>
-      <c r="AT31" s="26"/>
-      <c r="AU31" s="26"/>
-      <c r="AV31" s="26"/>
-      <c r="AW31" s="26"/>
-      <c r="AX31" s="26"/>
-      <c r="AY31" s="26"/>
-      <c r="AZ31" s="26"/>
+      <c r="U31" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="V31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="W31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="X31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH31" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI31" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ31" s="31"/>
+      <c r="AK31" s="31"/>
+      <c r="AL31" s="31"/>
+      <c r="AM31" s="31"/>
+      <c r="AN31" s="31"/>
+      <c r="AO31" s="31"/>
+      <c r="AP31" s="31"/>
+      <c r="AQ31" s="31"/>
+      <c r="AR31" s="31"/>
+      <c r="AS31" s="31"/>
+      <c r="AT31" s="31"/>
+      <c r="AU31" s="31"/>
+      <c r="AV31" s="31"/>
+      <c r="AW31" s="31"/>
+      <c r="AX31" s="31"/>
+      <c r="AY31" s="31"/>
+      <c r="AZ31" s="31"/>
     </row>
     <row r="32">
       <c r="A32" s="9" t="s">
@@ -4605,7 +4626,7 @@
       <c r="I32" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="17"/>
+      <c r="J32" s="21"/>
       <c r="K32" s="9" t="s">
         <v>44</v>
       </c>
@@ -4768,7 +4789,7 @@
         <v>43</v>
       </c>
       <c r="X33" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Y33" s="9" t="s">
         <v>43</v>
@@ -4911,7 +4932,7 @@
         <v>43</v>
       </c>
       <c r="AE34" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AF34" s="9" t="s">
         <v>43</v>
@@ -4969,7 +4990,7 @@
       <c r="I35" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J35" s="17"/>
+      <c r="J35" s="21"/>
       <c r="K35" s="9" t="s">
         <v>43</v>
       </c>
@@ -5007,7 +5028,7 @@
         <v>43</v>
       </c>
       <c r="W35" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X35" s="9" t="s">
         <v>43</v>
@@ -5089,7 +5110,7 @@
       <c r="I36" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J36" s="17"/>
+      <c r="J36" s="21"/>
       <c r="K36" s="9" t="s">
         <v>44</v>
       </c>
@@ -5127,7 +5148,7 @@
         <v>43</v>
       </c>
       <c r="W36" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X36" s="9" t="s">
         <v>43</v>
@@ -5136,7 +5157,7 @@
         <v>43</v>
       </c>
       <c r="Z36" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA36" s="9" t="s">
         <v>44</v>
@@ -5237,7 +5258,7 @@
         <v>43</v>
       </c>
       <c r="S37" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T37" s="9" t="s">
         <v>44</v>
@@ -5255,7 +5276,7 @@
         <v>43</v>
       </c>
       <c r="Y37" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z37" s="9" t="s">
         <v>44</v>
@@ -5344,7 +5365,7 @@
         <v>43</v>
       </c>
       <c r="N38" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O38" s="10" t="s">
         <v>44</v>
@@ -5362,7 +5383,7 @@
         <v>43</v>
       </c>
       <c r="T38" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U38" s="10" t="s">
         <v>44</v>
@@ -5371,7 +5392,7 @@
         <v>43</v>
       </c>
       <c r="W38" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X38" s="9" t="s">
         <v>43</v>
@@ -5490,7 +5511,7 @@
         <v>44</v>
       </c>
       <c r="V39" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W39" s="9" t="s">
         <v>44</v>
@@ -5514,7 +5535,7 @@
         <v>44</v>
       </c>
       <c r="AD39" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE39" s="9" t="s">
         <v>44</v>
@@ -5575,7 +5596,7 @@
       <c r="I40" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J40" s="17"/>
+      <c r="J40" s="21"/>
       <c r="K40" s="9" t="s">
         <v>44</v>
       </c>
@@ -5634,7 +5655,7 @@
         <v>44</v>
       </c>
       <c r="AD40" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE40" s="9" t="s">
         <v>44</v>
@@ -5646,7 +5667,7 @@
         <v>44</v>
       </c>
       <c r="AH40" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI40" s="9" t="s">
         <v>44</v>
@@ -5727,13 +5748,13 @@
         <v>43</v>
       </c>
       <c r="U41" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V41" s="9" t="s">
         <v>43</v>
       </c>
       <c r="W41" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X41" s="9" t="s">
         <v>43</v>
@@ -5742,7 +5763,7 @@
         <v>43</v>
       </c>
       <c r="Z41" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AA41" s="9" t="s">
         <v>43</v>
@@ -5754,7 +5775,7 @@
         <v>43</v>
       </c>
       <c r="AD41" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AE41" s="9" t="s">
         <v>43</v>
@@ -6116,10 +6137,10 @@
         <v>43</v>
       </c>
       <c r="AB44" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC44" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AD44" s="9" t="s">
         <v>44</v>
@@ -6134,7 +6155,7 @@
         <v>44</v>
       </c>
       <c r="AH44" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AI44" s="9" t="s">
         <v>44</v>
@@ -6183,7 +6204,7 @@
       <c r="I45" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="17"/>
+      <c r="J45" s="21"/>
       <c r="K45" s="9" t="s">
         <v>44</v>
       </c>
@@ -6227,7 +6248,7 @@
         <v>43</v>
       </c>
       <c r="Y45" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z45" s="9" t="s">
         <v>43</v>
@@ -6303,15 +6324,15 @@
       <c r="I46" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J46" s="17"/>
+      <c r="J46" s="21"/>
       <c r="K46" s="9" t="s">
         <v>43</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N46" s="9" t="s">
         <v>43</v>
@@ -6359,7 +6380,7 @@
         <v>43</v>
       </c>
       <c r="AC46" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AD46" s="9" t="s">
         <v>43</v>

</xml_diff>